<commit_message>
testiranje dodano, formatiranje popravljeno, grafovi
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -620,25 +620,180 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="2"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -848,6 +1003,27 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="2"/>
@@ -886,224 +1062,6 @@
         <top/>
         <bottom/>
         <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="2"/>
-        </left>
-        <right style="thin">
-          <color theme="2"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="2"/>
-        </vertical>
         <horizontal/>
       </border>
     </dxf>
@@ -1283,10 +1241,52 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1493,6 +1493,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>Zauzeće memorije</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1520,6 +1539,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$C$4:$C$18</c:f>
@@ -1595,6 +1668,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$D$4:$D$18</c:f>
@@ -1667,6 +1794,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$E$4:$E$18</c:f>
@@ -1736,6 +1917,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$F$4:$F$18</c:f>
@@ -1802,6 +2037,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$G$4:$G$18</c:f>
@@ -1865,6 +2154,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$H$4:$H$18</c:f>
@@ -1925,6 +2268,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$I$4:$I$18</c:f>
@@ -1982,6 +2379,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$J$4:$J$18</c:f>
@@ -2036,6 +2487,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$K$4:$K$18</c:f>
@@ -2087,6 +2592,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$L$4:$L$18</c:f>
@@ -2135,6 +2694,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$M$4:$M$18</c:f>
@@ -2180,6 +2793,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$N$4:$N$18</c:f>
@@ -2222,6 +2889,60 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$O$4:$O$18</c:f>
@@ -2250,21 +2971,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="42350080"/>
-        <c:axId val="173088768"/>
+        <c:axId val="152463232"/>
+        <c:axId val="152465408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42350080"/>
+        <c:axId val="152463232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:majorTickMark val="out"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173088768"/>
+        <c:crossAx val="152465408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2272,37 +3012,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173088768"/>
+        <c:axId val="152465408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>kB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42350080"/>
+        <c:crossAx val="152463232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2352,6 +3102,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$R$4:$R$18</c:f>
@@ -2425,6 +3229,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$S$4:$S$18</c:f>
@@ -2495,6 +3353,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$T$4:$T$18</c:f>
@@ -2562,6 +3474,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$U$4:$U$18</c:f>
@@ -2626,6 +3592,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$V$4:$V$18</c:f>
@@ -2687,6 +3707,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$W$4:$W$18</c:f>
@@ -2745,6 +3819,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$X$4:$X$18</c:f>
@@ -2800,6 +3928,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$Y$4:$Y$18</c:f>
@@ -2852,6 +4034,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$Z$4:$Z$18</c:f>
@@ -2901,6 +4137,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$AA$4:$AA$18</c:f>
@@ -2947,6 +4237,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$AB$4:$AB$18</c:f>
@@ -2990,6 +4334,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$AC$4:$AC$18</c:f>
@@ -3030,6 +4428,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$AD$4:$AD$18</c:f>
@@ -3060,20 +4512,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="41916672"/>
-        <c:axId val="41922560"/>
+        <c:axId val="152518016"/>
+        <c:axId val="152524288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41916672"/>
+        <c:axId val="152518016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41922560"/>
+        <c:crossAx val="152524288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3081,21 +4553,46 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41922560"/>
+        <c:axId val="152524288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>sekunda</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41916672"/>
+        <c:crossAx val="152518016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -3129,6 +4626,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>q=2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -3155,6 +4667,101 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'memory k=4'!$A$4:$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$C$4:$C$32</c:f>
@@ -3263,20 +4870,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82275712"/>
-        <c:axId val="173115648"/>
+        <c:axId val="153358336"/>
+        <c:axId val="153360256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82275712"/>
+        <c:axId val="153358336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173115648"/>
+        <c:crossAx val="153360256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3284,18 +4910,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173115648"/>
+        <c:axId val="153360256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>kB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82275712"/>
+        <c:crossAx val="153358336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3332,6 +4977,25 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>q=</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -3358,6 +5022,102 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'memory k=4'!$R$4:$R$32</c:f>
@@ -3466,20 +5226,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40832000"/>
-        <c:axId val="40872576"/>
+        <c:axId val="153397120"/>
+        <c:axId val="153399296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40832000"/>
+        <c:axId val="153397120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40872576"/>
+        <c:crossAx val="153399296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3487,18 +5267,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40872576"/>
+        <c:axId val="153399296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>sekunda</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40832000"/>
+        <c:crossAx val="153397120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3535,6 +5334,25 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>q=</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -3561,12 +5379,93 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$Q$4:$Q$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'memory k=4'!$S$4:$S$32</c:f>
+              <c:f>'memory k=4'!$S$4:$S$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3651,20 +5550,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43476480"/>
-        <c:axId val="43478016"/>
+        <c:axId val="153230336"/>
+        <c:axId val="153252992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43476480"/>
+        <c:axId val="153230336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43478016"/>
+        <c:crossAx val="153252992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3672,18 +5591,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43478016"/>
+        <c:axId val="153252992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>sekunda</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43476480"/>
+        <c:crossAx val="153230336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3720,6 +5658,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>q=3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -3734,11 +5687,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'memory k=4'!$C$3</c:f>
+              <c:f>'memory k=4'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3746,98 +5699,161 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'memory k=4'!$B$4:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'memory k=4'!$C$4:$C$32</c:f>
+              <c:f>'memory k=4'!$D$4:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>2904</c:v>
-                </c:pt>
+                <c:ptCount val="24"/>
                 <c:pt idx="1">
-                  <c:v>2808</c:v>
+                  <c:v>2684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2824</c:v>
+                  <c:v>2796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2872</c:v>
+                  <c:v>2896</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2832</c:v>
+                  <c:v>2916</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2824</c:v>
+                  <c:v>2956</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2852</c:v>
+                  <c:v>2948</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2904</c:v>
+                  <c:v>3004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2912</c:v>
+                  <c:v>2956</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2896</c:v>
+                  <c:v>3016</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2980</c:v>
+                  <c:v>3092</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2980</c:v>
+                  <c:v>3064</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3084</c:v>
+                  <c:v>3168</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3104</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3288</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3472</c:v>
+                  <c:v>3584</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3540</c:v>
+                  <c:v>3664</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3748</c:v>
+                  <c:v>3932</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3992</c:v>
+                  <c:v>4064</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4236</c:v>
+                  <c:v>4284</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4588</c:v>
+                  <c:v>4568</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4996</c:v>
+                  <c:v>5160</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5400</c:v>
+                  <c:v>5540</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5880</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6508</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6944</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7580</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8240</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9112</c:v>
+                  <c:v>5988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3854,20 +5870,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40364288"/>
-        <c:axId val="40521728"/>
+        <c:axId val="153261568"/>
+        <c:axId val="153263488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40364288"/>
+        <c:axId val="153261568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40521728"/>
+        <c:crossAx val="153263488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3875,18 +5911,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40521728"/>
+        <c:axId val="153263488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hr-HR"/>
+                  <a:t>kB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40364288"/>
+        <c:crossAx val="153261568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3913,15 +5968,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>598713</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>53746</xdr:rowOff>
+      <xdr:colOff>408214</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>340178</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>129946</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3943,15 +5998,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>544286</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>166007</xdr:rowOff>
+      <xdr:colOff>449036</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>102055</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4063,19 +6118,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>57829</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>148998</xdr:rowOff>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>343579</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>34698</xdr:rowOff>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>4082</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4108,9 +6163,9 @@
     <tableColumn id="9" name="9" dataDxfId="69"/>
     <tableColumn id="10" name="10" dataDxfId="68"/>
     <tableColumn id="11" name="11" dataDxfId="67"/>
-    <tableColumn id="15" name="12" dataDxfId="52"/>
-    <tableColumn id="14" name="13" dataDxfId="53"/>
-    <tableColumn id="13" name="14" dataDxfId="54"/>
+    <tableColumn id="15" name="12" dataDxfId="66"/>
+    <tableColumn id="14" name="13" dataDxfId="65"/>
+    <tableColumn id="13" name="14" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4119,6 +6174,71 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table5810" displayName="Table5810" ref="Q3:AD32" totalsRowShown="0">
   <autoFilter ref="Q3:AD32"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="-" dataDxfId="63"/>
+    <tableColumn id="2" name="2" dataDxfId="62"/>
+    <tableColumn id="3" name="3" dataDxfId="61"/>
+    <tableColumn id="4" name="4" dataDxfId="60"/>
+    <tableColumn id="5" name="5" dataDxfId="59"/>
+    <tableColumn id="6" name="6" dataDxfId="58"/>
+    <tableColumn id="7" name="7" dataDxfId="57"/>
+    <tableColumn id="8" name="8" dataDxfId="56"/>
+    <tableColumn id="9" name="9" dataDxfId="55"/>
+    <tableColumn id="10" name="10" dataDxfId="54"/>
+    <tableColumn id="11" name="11" dataDxfId="53"/>
+    <tableColumn id="15" name="12" dataDxfId="52"/>
+    <tableColumn id="14" name="13" dataDxfId="51"/>
+    <tableColumn id="13" name="14" dataDxfId="50"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="B3:M22" totalsRowShown="0">
+  <autoFilter ref="B3:M22"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="-" dataDxfId="49"/>
+    <tableColumn id="2" name="2" dataDxfId="48"/>
+    <tableColumn id="3" name="3" dataDxfId="47"/>
+    <tableColumn id="4" name="4" dataDxfId="46"/>
+    <tableColumn id="5" name="5" dataDxfId="45"/>
+    <tableColumn id="6" name="6" dataDxfId="44"/>
+    <tableColumn id="7" name="7" dataDxfId="43"/>
+    <tableColumn id="8" name="8" dataDxfId="42"/>
+    <tableColumn id="9" name="9" dataDxfId="41"/>
+    <tableColumn id="10" name="10" dataDxfId="40"/>
+    <tableColumn id="11" name="11" dataDxfId="39"/>
+    <tableColumn id="12" name="12" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table57911" displayName="Table57911" ref="O3:Z22" totalsRowShown="0">
+  <autoFilter ref="O3:Z22"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="-" dataDxfId="37"/>
+    <tableColumn id="2" name="2" dataDxfId="36"/>
+    <tableColumn id="3" name="3" dataDxfId="35"/>
+    <tableColumn id="4" name="4" dataDxfId="34"/>
+    <tableColumn id="5" name="5" dataDxfId="33"/>
+    <tableColumn id="6" name="6" dataDxfId="32"/>
+    <tableColumn id="7" name="7" dataDxfId="31"/>
+    <tableColumn id="8" name="8" dataDxfId="30"/>
+    <tableColumn id="9" name="9" dataDxfId="29"/>
+    <tableColumn id="10" name="10" dataDxfId="28"/>
+    <tableColumn id="11" name="11" dataDxfId="27"/>
+    <tableColumn id="12" name="12" dataDxfId="26"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table58" displayName="Table58" ref="B3:O22" totalsRowShown="0">
+  <autoFilter ref="B3:O22"/>
   <tableColumns count="14">
     <tableColumn id="1" name="-" dataDxfId="25"/>
     <tableColumn id="2" name="2" dataDxfId="24"/>
@@ -4139,30 +6259,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="B3:M22" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table579" displayName="Table579" ref="B3:M22" totalsRowShown="0">
   <autoFilter ref="B3:M22"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="-" dataDxfId="66"/>
-    <tableColumn id="2" name="2" dataDxfId="65"/>
-    <tableColumn id="3" name="3" dataDxfId="64"/>
-    <tableColumn id="4" name="4" dataDxfId="63"/>
-    <tableColumn id="5" name="5" dataDxfId="62"/>
-    <tableColumn id="6" name="6" dataDxfId="61"/>
-    <tableColumn id="7" name="7" dataDxfId="60"/>
-    <tableColumn id="8" name="8" dataDxfId="59"/>
-    <tableColumn id="9" name="9" dataDxfId="58"/>
-    <tableColumn id="10" name="10" dataDxfId="57"/>
-    <tableColumn id="11" name="11" dataDxfId="56"/>
-    <tableColumn id="12" name="12" dataDxfId="55"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table57911" displayName="Table57911" ref="O3:Z22" totalsRowShown="0">
-  <autoFilter ref="O3:Z22"/>
   <tableColumns count="12">
     <tableColumn id="1" name="-" dataDxfId="11"/>
     <tableColumn id="2" name="2" dataDxfId="10"/>
@@ -4176,50 +6275,6 @@
     <tableColumn id="10" name="10" dataDxfId="2"/>
     <tableColumn id="11" name="11" dataDxfId="1"/>
     <tableColumn id="12" name="12" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table58" displayName="Table58" ref="B3:O22" totalsRowShown="0">
-  <autoFilter ref="B3:O22"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="-" dataDxfId="26"/>
-    <tableColumn id="2" name="2" dataDxfId="51"/>
-    <tableColumn id="3" name="3" dataDxfId="50"/>
-    <tableColumn id="4" name="4" dataDxfId="49"/>
-    <tableColumn id="5" name="5" dataDxfId="48"/>
-    <tableColumn id="6" name="6" dataDxfId="47"/>
-    <tableColumn id="7" name="7" dataDxfId="46"/>
-    <tableColumn id="8" name="8" dataDxfId="45"/>
-    <tableColumn id="9" name="9" dataDxfId="44"/>
-    <tableColumn id="10" name="10" dataDxfId="43"/>
-    <tableColumn id="11" name="11" dataDxfId="42"/>
-    <tableColumn id="15" name="12" dataDxfId="41"/>
-    <tableColumn id="14" name="13" dataDxfId="40"/>
-    <tableColumn id="13" name="14" dataDxfId="39"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table579" displayName="Table579" ref="B3:M22" totalsRowShown="0">
-  <autoFilter ref="B3:M22"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="-" dataDxfId="27"/>
-    <tableColumn id="2" name="2" dataDxfId="38"/>
-    <tableColumn id="3" name="3" dataDxfId="37"/>
-    <tableColumn id="4" name="4" dataDxfId="36"/>
-    <tableColumn id="5" name="5" dataDxfId="35"/>
-    <tableColumn id="6" name="6" dataDxfId="34"/>
-    <tableColumn id="7" name="7" dataDxfId="33"/>
-    <tableColumn id="8" name="8" dataDxfId="32"/>
-    <tableColumn id="9" name="9" dataDxfId="31"/>
-    <tableColumn id="10" name="10" dataDxfId="30"/>
-    <tableColumn id="11" name="11" dataDxfId="29"/>
-    <tableColumn id="12" name="12" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4517,8 +6572,8 @@
   </sheetPr>
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U110" sqref="U110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>